<commit_message>
Correction of missing variables
Adding algorithms for:
smk_smoking_frequency
cog_dep_malaise 
sed_beh_tv_week_all
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-BCS.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-BCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD4B2B4-341A-4733-AF59-0CE7D0946E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED22E88-3129-4FFB-AD3E-866BF99D1EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{17FAC360-F975-4673-8378-999FF3470EEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{17FAC360-F975-4673-8378-999FF3470EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="449">
   <si>
     <t>index</t>
   </si>
@@ -1835,12 +1835,130 @@
   <si>
     <t>BCS_f1</t>
   </si>
+  <si>
+    <t>recode(3=1;4=2;ELSE=NA)</t>
+  </si>
+  <si>
+    <t>ifelse(bd11mal &gt;= 0, bd11mal, NA)</t>
+  </si>
+  <si>
+    <t>bd11mal</t>
+  </si>
+  <si>
+    <t>(Derived) Total Malaise score (9 questions)</t>
+  </si>
+  <si>
+    <t>HAM_Depression</t>
+  </si>
+  <si>
+    <t>(Derived) Total Malaise score (9 questions) . Derived from 9 self-reported questionnaire items.</t>
+  </si>
+  <si>
+    <t>Total malaise score from a 9 item short version of the malaise inventory (B10Q28A- B10Q28I). Items cover negative emotions and physical response and are coded so high malaise scores always relate to affirmative responses. The score is the total number of ‘yes’ responses meaning higher scores correspond to higher malaise. Cases were excluded if the number of items without a response accounted for scores being under 4 (the prerequisite score for high malaise).</t>
+  </si>
+  <si>
+    <t>-8=not enough information</t>
+  </si>
+  <si>
+    <t>Hours spent watching TV-weekday;
+Hours spent watching TV-weekend</t>
+  </si>
+  <si>
+    <t>RSB_TV</t>
+  </si>
+  <si>
+    <t>Hours spent watching TV-weekday. Self-reported questionnaire "How many hours do you spend watching television programmes, videos, DVDs or Blu-ray? Please include time spent watching programmes or films on a computer. a) On a typical weekday". Options were: None, Less than an hour a day, 1 to 2 hours a day, 2 to 3 hours a day, 3 to 4 hours a day, More than 4 hours a day;
+Hours spent watching TV-weekend. Self-reported questionnaire "How many hours do you spend watching television programmes, videos, DVDs or Blu-ray? Please include time spent watching programmes or films on a computer. b) On a typical day at the weekend". Options were: None, Less than an hour a day, 1 to 2 hours a day, 2 to 3 hours a day, 3 to 4 hours a day, More than 4 hours a day</t>
+  </si>
+  <si>
+    <t>-9=Not answered
+-8=Invalid answer, mulitple responses
+-1=Not applicable
+1=None
+2=Less than an hour a day
+3=1 to 2 hours a day
+4=2 to 3 hours a day
+5=3 to 4 hours a day
+6=More than 4 hours a day</t>
+  </si>
+  <si>
+    <t>b11q3a;
+b11q3b</t>
+  </si>
+  <si>
+    <t>case_when(
+(rowSums(mutate(.,
+temp_b11q3a = case_when(b11q3a == 1 ~ 0*5,
+b11q3a == 2 ~ 0.5*5,
+b11q3a == 3 ~ 1.5*5,
+b11q3a == 4 ~ 2.5*5,
+b11q3a == 5 ~ 3.5*5,
+b11q3a == 6 ~ 4*5,
+TRUE ~ NA_real_),
+temp_b11q3b = case_when(b11q3b == 1 ~ 0*2,
+b11q3b == 2 ~ 0.5*2,
+b11q3b == 3 ~ 1.5*2,
+b11q3b == 4 ~ 2.5*2,
+b11q3b == 5 ~ 3.5*2,
+b11q3b == 6 ~ 4*2,
+TRUE ~ NA_real_)) %&gt;%
+select(temp_b11q3a , temp_b11q3b), na.rm = FALSE)/7) &lt;= 1 ~ 1L;
+(rowSums(mutate(.,
+temp_b11q3a = case_when(b11q3a == 1 ~ 0*5,
+b11q3a == 2 ~ 0.5*5,
+b11q3a == 3 ~ 1.5*5,
+b11q3a == 4 ~ 2.5*5,
+b11q3a == 5 ~ 3.5*5,
+b11q3a == 6 ~ 4*5,
+TRUE ~ NA_real_),
+temp_b11q3b = case_when(b11q3b == 1 ~ 0*2,
+b11q3b == 2 ~ 0.5*2,
+b11q3b == 3 ~ 1.5*2,
+b11q3b == 4 ~ 2.5*2,
+b11q3b == 5 ~ 3.5*2,
+b11q3b == 6 ~ 4*2,
+TRUE ~ NA_real_)) %&gt;%
+select(temp_b11q3a , temp_b11q3b), na.rm = FALSE)/7) &gt; 1 &amp;
+(rowSums(mutate(.,
+temp_b11q3a = case_when(b11q3a == 1 ~ 0*5,
+b11q3a == 2 ~ 0.5*5,
+b11q3a == 3 ~ 1.5*5,
+b11q3a == 4 ~ 2.5*5,
+b11q3a == 5 ~ 3.5*5,
+b11q3a == 6 ~ 4*5,
+TRUE ~ NA_real_),
+temp_b11q3b = case_when(b11q3b == 1 ~ 0*2,
+b11q3b == 2 ~ 0.5*2,
+b11q3b == 3 ~ 1.5*2,
+b11q3b == 4 ~ 2.5*2,
+b11q3b == 5 ~ 3.5*2,
+b11q3b == 6 ~ 4*2,
+TRUE ~ NA_real_)) %&gt;%
+select(temp_b11q3a , temp_b11q3b), na.rm = FALSE)/7) &lt;= 3 ~ 2L;
+(rowSums(mutate(.,
+temp_b11q3a = case_when(b11q3a == 1 ~ 0*5,
+b11q3a == 2 ~ 0.5*5,
+b11q3a == 3 ~ 1.5*5,
+b11q3a == 4 ~ 2.5*5,
+b11q3a == 5 ~ 3.5*5,
+b11q3a == 6 ~ 4*5,
+TRUE ~ NA_real_),
+temp_b11q3b = case_when(b11q3b == 1 ~ 0*2,
+b11q3b == 2 ~ 0.5*2,
+b11q3b == 3 ~ 1.5*2,
+b11q3b == 4 ~ 2.5*2,
+b11q3b == 5 ~ 3.5*2,
+b11q3b == 6 ~ 4*2,
+TRUE ~ NA_real_)) %&gt;%
+select(temp_b11q3a , temp_b11q3b), na.rm = FALSE)/7) &gt; 3 ~ 3L; 
+ELSE ~ NA_integer_)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1848,19 +1966,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1875,14 +1993,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1901,7 +2024,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2219,12 +2342,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9A9556-6A71-4D41-957B-24579A577B61}">
   <dimension ref="A1:AD167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D84" sqref="D84"/>
+      <selection pane="topRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" customWidth="1"/>
@@ -2237,7 +2360,7 @@
     <col min="17" max="17" width="41.42578125" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" customWidth="1"/>
     <col min="22" max="22" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="61.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="61.42578125" style="4" customWidth="1"/>
     <col min="24" max="24" width="14.5703125" customWidth="1"/>
     <col min="25" max="25" width="23.5703125" customWidth="1"/>
     <col min="26" max="26" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -2310,7 +2433,7 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
@@ -2384,7 +2507,7 @@
       <c r="V2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2419,7 +2542,7 @@
       <c r="V3" t="s">
         <v>47</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="4">
         <v>2</v>
       </c>
     </row>
@@ -2481,7 +2604,7 @@
       <c r="V4" t="s">
         <v>61</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2531,7 +2654,7 @@
       <c r="V5" t="s">
         <v>70</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2587,7 +2710,7 @@
       <c r="V6" t="s">
         <v>47</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="4">
         <v>51</v>
       </c>
     </row>
@@ -2631,7 +2754,7 @@
       <c r="V7" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2675,7 +2798,7 @@
       <c r="V8" t="s">
         <v>70</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2719,7 +2842,7 @@
       <c r="V9" t="s">
         <v>70</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="W9" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2754,7 +2877,7 @@
       <c r="V10" t="s">
         <v>101</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2810,7 +2933,7 @@
       <c r="V11" t="s">
         <v>70</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="4" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2854,7 +2977,7 @@
       <c r="V12" t="s">
         <v>70</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2910,7 +3033,7 @@
       <c r="V13" t="s">
         <v>70</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="W13" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2963,7 +3086,7 @@
       <c r="V14" t="s">
         <v>70</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="W14" s="4" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3007,7 +3130,7 @@
       <c r="V15" t="s">
         <v>70</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="W15" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3048,7 +3171,7 @@
       <c r="V16" t="s">
         <v>141</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="W16" s="4" t="s">
         <v>142</v>
       </c>
       <c r="Z16" t="s">
@@ -3092,7 +3215,7 @@
       <c r="V17" t="s">
         <v>141</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W17" s="4" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3136,7 +3259,7 @@
       <c r="V18" t="s">
         <v>141</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="W18" s="4" t="s">
         <v>150</v>
       </c>
       <c r="Z18" t="s">
@@ -3183,7 +3306,7 @@
       <c r="V19" t="s">
         <v>141</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="W19" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3227,7 +3350,7 @@
       <c r="V20" t="s">
         <v>141</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="W20" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3265,7 +3388,7 @@
       <c r="V21" t="s">
         <v>101</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="W21" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3303,7 +3426,7 @@
       <c r="V22" t="s">
         <v>101</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="W22" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3341,7 +3464,7 @@
       <c r="V23" t="s">
         <v>101</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="W23" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3376,7 +3499,7 @@
       <c r="V24" t="s">
         <v>101</v>
       </c>
-      <c r="W24" s="1" t="s">
+      <c r="W24" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3414,7 +3537,7 @@
       <c r="V25" t="s">
         <v>101</v>
       </c>
-      <c r="W25" s="1" t="s">
+      <c r="W25" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3452,7 +3575,7 @@
       <c r="V26" t="s">
         <v>101</v>
       </c>
-      <c r="W26" s="1" t="s">
+      <c r="W26" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3490,7 +3613,7 @@
       <c r="V27" t="s">
         <v>101</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="W27" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3528,7 +3651,7 @@
       <c r="V28" t="s">
         <v>101</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="W28" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3566,7 +3689,7 @@
       <c r="V29" t="s">
         <v>101</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="W29" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3604,7 +3727,7 @@
       <c r="V30" t="s">
         <v>101</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="W30" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3642,7 +3765,7 @@
       <c r="V31" t="s">
         <v>101</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="W31" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3680,7 +3803,7 @@
       <c r="V32" t="s">
         <v>101</v>
       </c>
-      <c r="W32" s="1" t="s">
+      <c r="W32" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3718,7 +3841,7 @@
       <c r="V33" t="s">
         <v>101</v>
       </c>
-      <c r="W33" s="1" t="s">
+      <c r="W33" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3756,7 +3879,7 @@
       <c r="V34" t="s">
         <v>101</v>
       </c>
-      <c r="W34" s="1" t="s">
+      <c r="W34" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3794,7 +3917,7 @@
       <c r="V35" t="s">
         <v>101</v>
       </c>
-      <c r="W35" s="1" t="s">
+      <c r="W35" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3832,7 +3955,7 @@
       <c r="V36" t="s">
         <v>101</v>
       </c>
-      <c r="W36" s="1" t="s">
+      <c r="W36" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3870,7 +3993,7 @@
       <c r="V37" t="s">
         <v>101</v>
       </c>
-      <c r="W37" s="1" t="s">
+      <c r="W37" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3908,7 +4031,7 @@
       <c r="V38" t="s">
         <v>101</v>
       </c>
-      <c r="W38" s="1" t="s">
+      <c r="W38" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3946,7 +4069,7 @@
       <c r="V39" t="s">
         <v>101</v>
       </c>
-      <c r="W39" s="1" t="s">
+      <c r="W39" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3984,7 +4107,7 @@
       <c r="V40" t="s">
         <v>101</v>
       </c>
-      <c r="W40" s="1" t="s">
+      <c r="W40" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4022,7 +4145,7 @@
       <c r="V41" t="s">
         <v>101</v>
       </c>
-      <c r="W41" s="1" t="s">
+      <c r="W41" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4060,7 +4183,7 @@
       <c r="V42" t="s">
         <v>101</v>
       </c>
-      <c r="W42" s="1" t="s">
+      <c r="W42" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4098,7 +4221,7 @@
       <c r="V43" t="s">
         <v>101</v>
       </c>
-      <c r="W43" t="s">
+      <c r="W43" s="5" t="s">
         <v>101</v>
       </c>
       <c r="X43" t="s">
@@ -4148,7 +4271,7 @@
       <c r="V44" t="s">
         <v>70</v>
       </c>
-      <c r="W44" s="1" t="s">
+      <c r="W44" s="4" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4201,11 +4324,11 @@
       <c r="V45" t="s">
         <v>70</v>
       </c>
-      <c r="W45" s="1" t="s">
+      <c r="W45" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="225" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4228,19 +4351,31 @@
         <v>218</v>
       </c>
       <c r="J46" t="s">
-        <v>46</v>
+        <v>211</v>
+      </c>
+      <c r="K46" t="s">
+        <v>212</v>
+      </c>
+      <c r="L46" t="s">
+        <v>213</v>
+      </c>
+      <c r="M46" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="T46" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="U46" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="V46" t="s">
-        <v>101</v>
-      </c>
-      <c r="W46" s="1" t="s">
-        <v>101</v>
+        <v>70</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -4292,7 +4427,7 @@
       <c r="V47" t="s">
         <v>61</v>
       </c>
-      <c r="W47" s="1" t="s">
+      <c r="W47" s="4" t="s">
         <v>341</v>
       </c>
     </row>
@@ -4336,7 +4471,7 @@
       <c r="V48" t="s">
         <v>70</v>
       </c>
-      <c r="W48" s="1" t="s">
+      <c r="W48" s="4" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4380,7 +4515,7 @@
       <c r="V49" t="s">
         <v>141</v>
       </c>
-      <c r="W49" s="1" t="s">
+      <c r="W49" s="4" t="s">
         <v>342</v>
       </c>
       <c r="X49" t="s">
@@ -4424,7 +4559,7 @@
       <c r="V50" t="s">
         <v>101</v>
       </c>
-      <c r="W50" s="1" t="s">
+      <c r="W50" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4465,7 +4600,7 @@
       <c r="V51" t="s">
         <v>70</v>
       </c>
-      <c r="W51" s="1" t="s">
+      <c r="W51" s="4" t="s">
         <v>330</v>
       </c>
     </row>
@@ -4503,7 +4638,7 @@
       <c r="V52" t="s">
         <v>101</v>
       </c>
-      <c r="W52" s="1" t="s">
+      <c r="W52" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4544,7 +4679,7 @@
       <c r="V53" t="s">
         <v>70</v>
       </c>
-      <c r="W53" s="1" t="s">
+      <c r="W53" s="4" t="s">
         <v>330</v>
       </c>
       <c r="X53" s="1" t="s">
@@ -4591,7 +4726,7 @@
       <c r="V54" t="s">
         <v>70</v>
       </c>
-      <c r="W54" s="1" t="s">
+      <c r="W54" s="4" t="s">
         <v>330</v>
       </c>
       <c r="X54" t="s">
@@ -4635,7 +4770,7 @@
       <c r="V55" t="s">
         <v>101</v>
       </c>
-      <c r="W55" s="1" t="s">
+      <c r="W55" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4673,7 +4808,7 @@
       <c r="V56" t="s">
         <v>101</v>
       </c>
-      <c r="W56" s="1" t="s">
+      <c r="W56" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4711,7 +4846,7 @@
       <c r="V57" t="s">
         <v>101</v>
       </c>
-      <c r="W57" s="1" t="s">
+      <c r="W57" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4749,7 +4884,7 @@
       <c r="V58" t="s">
         <v>101</v>
       </c>
-      <c r="W58" s="1" t="s">
+      <c r="W58" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4784,7 +4919,7 @@
       <c r="V59" t="s">
         <v>101</v>
       </c>
-      <c r="W59" s="1" t="s">
+      <c r="W59" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4819,7 +4954,7 @@
       <c r="V60" t="s">
         <v>101</v>
       </c>
-      <c r="W60" s="1" t="s">
+      <c r="W60" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4843,19 +4978,38 @@
         <v>45</v>
       </c>
       <c r="J61" t="s">
-        <v>46</v>
+        <v>437</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>442</v>
       </c>
       <c r="T61" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="U61" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="V61" t="s">
-        <v>101</v>
-      </c>
-      <c r="W61" s="1" t="s">
-        <v>101</v>
+        <v>61</v>
+      </c>
+      <c r="W61" s="5" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
@@ -4889,7 +5043,7 @@
       <c r="V62" t="s">
         <v>101</v>
       </c>
-      <c r="W62" s="1" t="s">
+      <c r="W62" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4924,7 +5078,7 @@
       <c r="V63" t="s">
         <v>101</v>
       </c>
-      <c r="W63" s="1" t="s">
+      <c r="W63" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4959,7 +5113,7 @@
       <c r="V64" t="s">
         <v>101</v>
       </c>
-      <c r="W64" s="1" t="s">
+      <c r="W64" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4994,7 +5148,7 @@
       <c r="V65" t="s">
         <v>101</v>
       </c>
-      <c r="W65" s="1" t="s">
+      <c r="W65" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5032,7 +5186,7 @@
       <c r="V66" t="s">
         <v>101</v>
       </c>
-      <c r="W66" s="1" t="s">
+      <c r="W66" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5073,7 +5227,7 @@
       <c r="V67" t="s">
         <v>61</v>
       </c>
-      <c r="W67" s="1" t="s">
+      <c r="W67" s="4" t="s">
         <v>347</v>
       </c>
     </row>
@@ -5114,7 +5268,7 @@
       <c r="V68" t="s">
         <v>141</v>
       </c>
-      <c r="W68" s="1" t="s">
+      <c r="W68" s="4" t="s">
         <v>348</v>
       </c>
     </row>
@@ -5167,11 +5321,11 @@
       <c r="V69" t="s">
         <v>101</v>
       </c>
-      <c r="W69" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+      <c r="W69" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5193,20 +5347,39 @@
       <c r="I70" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="J70" t="s">
-        <v>46</v>
-      </c>
-      <c r="T70" t="s">
-        <v>101</v>
-      </c>
-      <c r="U70" t="s">
-        <v>273</v>
-      </c>
-      <c r="V70" t="s">
-        <v>101</v>
-      </c>
-      <c r="W70" s="1" t="s">
-        <v>101</v>
+      <c r="J70" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q70" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2"/>
+      <c r="T70" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="285" x14ac:dyDescent="0.25">
@@ -5255,7 +5428,7 @@
       <c r="V71" t="s">
         <v>70</v>
       </c>
-      <c r="W71" s="1" t="s">
+      <c r="W71" s="4" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5305,7 +5478,7 @@
       <c r="V72" t="s">
         <v>70</v>
       </c>
-      <c r="W72" s="1" t="s">
+      <c r="W72" s="4" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5343,7 +5516,7 @@
       <c r="V73" t="s">
         <v>101</v>
       </c>
-      <c r="W73" s="1" t="s">
+      <c r="W73" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5381,7 +5554,7 @@
       <c r="V74" t="s">
         <v>101</v>
       </c>
-      <c r="W74" s="1" t="s">
+      <c r="W74" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5419,7 +5592,7 @@
       <c r="V75" t="s">
         <v>101</v>
       </c>
-      <c r="W75" s="1" t="s">
+      <c r="W75" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5457,7 +5630,7 @@
       <c r="V76" t="s">
         <v>101</v>
       </c>
-      <c r="W76" s="1" t="s">
+      <c r="W76" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5495,7 +5668,7 @@
       <c r="V77" t="s">
         <v>101</v>
       </c>
-      <c r="W77" s="1" t="s">
+      <c r="W77" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5539,7 +5712,7 @@
       <c r="V78" t="s">
         <v>70</v>
       </c>
-      <c r="W78" s="1" t="s">
+      <c r="W78" s="4" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5583,7 +5756,7 @@
       <c r="V79" t="s">
         <v>70</v>
       </c>
-      <c r="W79" s="1" t="s">
+      <c r="W79" s="4" t="s">
         <v>302</v>
       </c>
     </row>
@@ -5621,7 +5794,7 @@
       <c r="V80" t="s">
         <v>141</v>
       </c>
-      <c r="W80" s="1" t="s">
+      <c r="W80" s="4" t="s">
         <v>306</v>
       </c>
     </row>
@@ -5665,7 +5838,7 @@
       <c r="V81" t="s">
         <v>141</v>
       </c>
-      <c r="W81" s="1" t="s">
+      <c r="W81" s="4" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5703,7 +5876,7 @@
       <c r="V82" t="s">
         <v>141</v>
       </c>
-      <c r="W82" s="1" t="s">
+      <c r="W82" s="4" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5741,7 +5914,7 @@
       <c r="V83" t="s">
         <v>61</v>
       </c>
-      <c r="W83" s="1" t="s">
+      <c r="W83" s="4" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5779,7 +5952,7 @@
       <c r="V84" t="s">
         <v>61</v>
       </c>
-      <c r="W84" s="1" t="s">
+      <c r="W84" s="4" t="s">
         <v>351</v>
       </c>
     </row>
@@ -5793,7 +5966,6 @@
       <c r="M87" s="1"/>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
-      <c r="W87" s="2"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I88" s="1"/>
@@ -5823,41 +5995,39 @@
       <c r="M96" s="1"/>
       <c r="Q96" s="1"/>
     </row>
-    <row r="97" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I97" s="1"/>
       <c r="M97" s="1"/>
       <c r="Q97" s="1"/>
     </row>
-    <row r="98" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I98" s="1"/>
       <c r="Q98" s="1"/>
     </row>
-    <row r="99" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:17" x14ac:dyDescent="0.25">
       <c r="J99" s="1"/>
       <c r="P99" s="1"/>
-      <c r="W99" s="2"/>
-    </row>
-    <row r="100" spans="9:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
       <c r="P100" s="1"/>
     </row>
-    <row r="101" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:17" x14ac:dyDescent="0.25">
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="P101" s="1"/>
-      <c r="W101" s="2"/>
-    </row>
-    <row r="102" spans="9:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="P102" s="1"/>
     </row>
-    <row r="105" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I105" s="1"/>
     </row>
-    <row r="112" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I112" s="1"/>
     </row>
     <row r="122" spans="9:23" x14ac:dyDescent="0.25">
@@ -5868,7 +6038,7 @@
     </row>
     <row r="126" spans="9:23" x14ac:dyDescent="0.25">
       <c r="J126" s="1"/>
-      <c r="W126"/>
+      <c r="W126" s="5"/>
     </row>
     <row r="127" spans="9:23" x14ac:dyDescent="0.25">
       <c r="I127" s="1"/>
@@ -6002,5 +6172,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>